<commit_message>
Simulations vignette with references to all configuration files and first lines of output
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Code/ProjectConfiguration.xlsx
+++ b/tests/data/TestProject/Code/ProjectConfiguration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svavil\Downloads\esqlabs\esqlabsR\tests\data\TestProject\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D127FC-B74A-40DB-86C4-720FF6961C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041F5FB9-CEB9-4493-9E1C-BAF66D8C1024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -147,10 +147,10 @@
     <t>ApplicationParameters.xlsx</t>
   </si>
   <si>
-    <t>../..</t>
-  </si>
-  <si>
     <t>TestProject_TimeValuesData.xlsx</t>
+  </si>
+  <si>
+    <t>../Models</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -480,17 +480,17 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.59765625" customWidth="1"/>
-    <col min="2" max="2" width="38.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6328125" customWidth="1"/>
+    <col min="2" max="2" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,18 +501,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -523,7 +523,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -534,7 +534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -545,7 +545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -556,7 +556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -567,7 +567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -578,7 +578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -589,7 +589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -600,18 +600,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -622,7 +622,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -633,7 +633,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -651,15 +651,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6d50ae52c45ae5cf3a9b42a45f9049e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f65cf74c317ca0ec831fcb171d38ef6f" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -876,6 +867,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -883,14 +883,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE9E921-488E-4950-83CF-BA07CBEDBDF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -909,6 +901,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Rename `IndividualPhysiology.xlsx` to `IndividualBiometrics.xlsx`
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Code/ProjectConfiguration.xlsx
+++ b/tests/data/TestProject/Code/ProjectConfiguration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\esqlabsR\tests\data\TestProject\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04E4FEB-FF97-4B01-94A4-77891EC62029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2743BAE3-0502-4EBA-BFA5-9FF48537EA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>IndividualParameters.xlsx</t>
   </si>
   <si>
-    <t>IndividualPhysiology.xlsx</t>
-  </si>
-  <si>
     <t>individualPhysiologyFile</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Name of the excel file with individual-specific model parametrization. Must be located in the "paramsFolder"</t>
   </si>
   <si>
-    <t>Name of the excel file with individual physiology information. Must be located in the "paramsFolder"</t>
-  </si>
-  <si>
     <t>populationParamsFile</t>
   </si>
   <si>
@@ -160,6 +154,12 @@
   </si>
   <si>
     <t>Name of the excel file with plot definitions. Must be located in the "paramsFolder"</t>
+  </si>
+  <si>
+    <t>IndividualBiometrics.xlsx</t>
+  </si>
+  <si>
+    <t>Name of the excel file with individual biometrics information. Must be located in the "paramsFolder"</t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -489,17 +489,17 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5859375" customWidth="1"/>
-    <col min="2" max="2" width="38.05859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.5859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,21 +507,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -529,10 +529,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -540,128 +540,128 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -671,6 +671,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6d50ae52c45ae5cf3a9b42a45f9049e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f65cf74c317ca0ec831fcb171d38ef6f" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -887,22 +902,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE9E921-488E-4950-83CF-BA07CBEDBDF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -919,21 +936,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>